<commit_message>
Figuring out grid Layout
</commit_message>
<xml_diff>
--- a/Roll20/CharacterSheet/GridLayout.xlsx
+++ b/Roll20/CharacterSheet/GridLayout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repository\GitHub\Adelphia\Roll20\CharacterSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9396EE73-C4DE-4E42-A1CB-829BF2E043D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64C86C5-8858-42F3-A23A-8CCC21653C60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{E0D01542-689A-4A2E-B27C-8B80433C7E51}"/>
   </bookViews>
@@ -50,12 +50,6 @@
     <t>Riposte Stats</t>
   </si>
   <si>
-    <t>Character Picture</t>
-  </si>
-  <si>
-    <t>Aspect List</t>
-  </si>
-  <si>
     <t>Character</t>
   </si>
   <si>
@@ -87,13 +81,20 @@
   </si>
   <si>
     <t>Growth Per Level</t>
+  </si>
+  <si>
+    <t>Character
+Picture</t>
+  </si>
+  <si>
+    <t>Quirks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,20 +102,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,15 +129,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -454,109 +457,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9A71EF-9A41-4B00-B52D-71CA1FC46C79}">
-  <dimension ref="B1:L5"/>
+  <dimension ref="B1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.26953125" style="1"/>
+    <col min="1" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="J1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2"/>
     </row>
+    <row r="6" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>